<commit_message>
Add Saturn and Uranus
</commit_message>
<xml_diff>
--- a/Sonnensystem Fakten.xlsx
+++ b/Sonnensystem Fakten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Computergrafik und Animation\Prj_OuterSpace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3A85328-0FDB-4085-AB4F-6D77186E5505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CADD92-999D-496E-81D0-6E447A964EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="3150" windowWidth="21600" windowHeight="11325" xr2:uid="{AF2B4829-EF71-49F6-AB5B-12C26267CF5D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Venus</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Abstand zur sonne (in Mio. KM)</t>
+  </si>
+  <si>
+    <t>Abstand bei uns</t>
   </si>
 </sst>
 </file>
@@ -482,19 +485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C45116-BC61-4783-9D9F-E01E507F450E}">
-  <dimension ref="B3:E12"/>
+  <dimension ref="B3:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -502,37 +505,42 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
         <v>109</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>57.9</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
         <v>0.38300000000000001</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -540,13 +548,16 @@
         <v>108.2</v>
       </c>
       <c r="D6" s="3">
+        <v>80</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.95</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -554,13 +565,16 @@
         <v>149.6</v>
       </c>
       <c r="D7" s="3">
+        <v>149</v>
+      </c>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -568,25 +582,31 @@
         <v>227.9</v>
       </c>
       <c r="D8" s="3">
+        <v>227</v>
+      </c>
+      <c r="E8" s="3">
         <v>0.53300000000000003</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5">
         <v>779</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
+        <v>300</v>
+      </c>
+      <c r="E9" s="3">
         <v>11.2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -594,13 +614,16 @@
         <v>1433</v>
       </c>
       <c r="D10" s="3">
+        <v>400</v>
+      </c>
+      <c r="E10" s="3">
         <v>9.41</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -608,21 +631,25 @@
         <v>2871</v>
       </c>
       <c r="D11" s="3">
+        <v>520</v>
+      </c>
+      <c r="E11" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3">
         <v>4495</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
         <v>3.8</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>